<commit_message>
fixed loader for weights path
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ninja\School\Atari-Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AD9FBE-5BFF-4EE1-AB56-E78946F957C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE80DDEF-6530-43D8-B660-4DDFEED18C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{F056FDBC-FD1C-4AAD-B5EB-AB9B4822F501}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F056FDBC-FD1C-4AAD-B5EB-AB9B4822F501}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>HOURS</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>reorganized code/folders and tried to add commits</t>
+  </si>
+  <si>
+    <t>created this, talked o you, and more</t>
+  </si>
+  <si>
+    <t>pips: gymnasium, ale_py, torch,</t>
+  </si>
+  <si>
+    <t>meeting with prof.</t>
   </si>
 </sst>
 </file>
@@ -112,7 +121,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[h]:mm"/>
+    <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -145,7 +154,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -481,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA24217B-B1AF-4ADA-826D-205E5762FA65}">
-  <dimension ref="A2:M18"/>
+  <dimension ref="A2:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,7 +546,7 @@
       </c>
       <c r="M4" s="1">
         <f>SUM(C:C)</f>
-        <v>1.4930555555555554</v>
+        <v>1.5486111111111109</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -555,7 +564,7 @@
       </c>
       <c r="M5" s="1">
         <f>M3-M4</f>
-        <v>2.2569444444444446</v>
+        <v>2.2013888888888893</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -699,6 +708,33 @@
       </c>
       <c r="E18" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>45994</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>46000</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>